<commit_message>
Started progress on final Clemens comments
</commit_message>
<xml_diff>
--- a/pockels rotations contrast figure/pockels-rotations.xlsx
+++ b/pockels rotations contrast figure/pockels-rotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carcu\Documents\PhD\thesis 2\pockels rotations contrast figure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E194A06F-6DE4-48BB-86D3-5F94028D8BD0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E86AC1F-3105-4BDA-9970-9398019D8933}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12165" xr2:uid="{4BEF3F0B-F16B-4F81-9DAB-4D2AC30286F2}"/>
   </bookViews>
@@ -105,12 +105,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -228,31 +228,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0.84379999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0.89459999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0.80269999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -342,31 +342,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.92</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98</c:v>
+                  <c:v>0.99680000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.95</c:v>
+                  <c:v>0.97570000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.99680000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.97570000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,31 +456,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0.94059999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0.96799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0.95279999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,16 +1297,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1634,34 +1634,34 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
       <c r="T1" t="s">
         <v>2</v>
       </c>
@@ -1679,36 +1679,36 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>488</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4">
         <v>561</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4">
         <v>640</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4">
         <v>488</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4">
         <v>561</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1">
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4">
         <v>640</v>
       </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
       <c r="T2" t="s">
         <v>0</v>
       </c>
@@ -1716,113 +1716,113 @@
         <v>0</v>
       </c>
       <c r="V2">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="W2">
-        <v>0.92</v>
+        <v>0.78</v>
       </c>
       <c r="X2">
-        <v>0.5</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>60</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>120</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>60</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>120</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>60</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>120</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>0</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>60</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <v>120</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>0</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>60</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <v>120</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <v>0</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="1">
         <v>60</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="1">
         <v>120</v>
       </c>
       <c r="U3">
         <v>60</v>
       </c>
       <c r="V3">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="W3">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="X3">
-        <v>0.5</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
       <c r="U4">
         <v>120</v>
       </c>
       <c r="V4">
-        <v>0.5</v>
+        <v>0.13</v>
       </c>
       <c r="W4">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="X4">
-        <v>0.5</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1833,13 +1833,13 @@
         <v>0</v>
       </c>
       <c r="V5">
-        <v>0.5</v>
+        <v>0.84379999999999999</v>
       </c>
       <c r="W5">
-        <v>0.98</v>
+        <v>0.99680000000000002</v>
       </c>
       <c r="X5">
-        <v>0.5</v>
+        <v>0.94059999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1847,13 +1847,13 @@
         <v>60</v>
       </c>
       <c r="V6">
-        <v>0.5</v>
+        <v>0.89459999999999995</v>
       </c>
       <c r="W6">
-        <v>0.95</v>
+        <v>0.97570000000000001</v>
       </c>
       <c r="X6">
-        <v>0.5</v>
+        <v>0.96799999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -1861,13 +1861,13 @@
         <v>120</v>
       </c>
       <c r="V7">
-        <v>0.5</v>
+        <v>0.80269999999999997</v>
       </c>
       <c r="W7">
         <v>1</v>
       </c>
       <c r="X7">
-        <v>0.5</v>
+        <v>0.95279999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1878,13 +1878,13 @@
         <v>0</v>
       </c>
       <c r="V8">
-        <v>0.5</v>
+        <v>0.78</v>
       </c>
       <c r="W8">
-        <v>0.5</v>
+        <v>0.99680000000000002</v>
       </c>
       <c r="X8">
-        <v>0.5</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1892,13 +1892,13 @@
         <v>60</v>
       </c>
       <c r="V9">
-        <v>0.5</v>
+        <v>0.67</v>
       </c>
       <c r="W9">
-        <v>0.5</v>
+        <v>0.97570000000000001</v>
       </c>
       <c r="X9">
-        <v>0.5</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1906,17 +1906,17 @@
         <v>120</v>
       </c>
       <c r="V10">
-        <v>0.5</v>
+        <v>0.79</v>
       </c>
       <c r="W10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="U12" s="4"/>
+      <c r="U12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>